<commit_message>
masukan data peserta untuk seleksi
</commit_message>
<xml_diff>
--- a/pesertaseleksidb.xlsx
+++ b/pesertaseleksidb.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\mikroskil\kmkmikroskil\2015\pansel\seleksi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2. Janward Alfredo Situmorang\KMK\KMK 2015\PanselFolder\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
   <si>
     <t>Daftar Peserta Seleksi Pengurus UKM - KMK Mikroskil Medan Periode 2015/2016</t>
   </si>
@@ -155,6 +155,12 @@
   </si>
   <si>
     <t>TI (2014)</t>
+  </si>
+  <si>
+    <t>Sabtu 4 Juli 2015</t>
+  </si>
+  <si>
+    <t>Jumat 3 Juli 2015</t>
   </si>
 </sst>
 </file>
@@ -242,7 +248,134 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -253,6 +386,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:E29" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A4:E29"/>
+  <tableColumns count="5">
+    <tableColumn id="1" name="NIM" dataDxfId="6"/>
+    <tableColumn id="2" name="Nama" dataDxfId="5"/>
+    <tableColumn id="3" name="E-mail" dataDxfId="4"/>
+    <tableColumn id="4" name="CP" dataDxfId="3"/>
+    <tableColumn id="5" name="Tanggal Seleksi I" dataDxfId="2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -656,8 +803,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -762,74 +909,80 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="2:2" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="2:2" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="2:2" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="20" spans="2:2" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="2:2" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="22" spans="2:2" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="23" spans="2:2" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="24" spans="2:2" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B24" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="25" spans="2:2" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="2" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="26" spans="2:2" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E25" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="26" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="2" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="27" spans="2:2" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E26" s="2" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="27" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="28" spans="2:2" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="29" spans="2:2" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="30" spans="2:2" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:2" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:2" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="30" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="31" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="33" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="34" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="35" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -858,6 +1011,9 @@
     <row r="58" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
penambahan data yang masuk pada peserta seleksi
</commit_message>
<xml_diff>
--- a/pesertaseleksidb.xlsx
+++ b/pesertaseleksidb.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="53">
   <si>
     <t>Daftar Peserta Seleksi Pengurus UKM - KMK Mikroskil Medan Periode 2015/2016</t>
   </si>
@@ -94,9 +94,6 @@
     <t>Immanuel Sembiring</t>
   </si>
   <si>
-    <t>Didik</t>
-  </si>
-  <si>
     <t>Samuel Simanungkalit</t>
   </si>
   <si>
@@ -161,13 +158,40 @@
   </si>
   <si>
     <t>Jumat 3 Juli 2015</t>
+  </si>
+  <si>
+    <t>Herbet Hutagalung</t>
+  </si>
+  <si>
+    <t>Sabtu 04 Juli 2015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Eva </t>
+  </si>
+  <si>
+    <t>SI (2014)</t>
+  </si>
+  <si>
+    <t>Mutiara Novi Tamara Ginting</t>
+  </si>
+  <si>
+    <t>Lidya Veronica Hutabarat</t>
+  </si>
+  <si>
+    <t>082166562468</t>
+  </si>
+  <si>
+    <t>085762395411</t>
+  </si>
+  <si>
+    <t>Riddik</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -206,6 +230,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -228,7 +258,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -243,12 +273,284 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="21">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -389,8 +691,45 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:E29" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:E29" totalsRowShown="0" headerRowDxfId="7" dataDxfId="8">
   <autoFilter ref="A4:E29"/>
+  <sortState ref="A5:E29">
+    <sortCondition ref="B4:B29"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="1" name="NIM" dataDxfId="13"/>
+    <tableColumn id="2" name="Nama" dataDxfId="12"/>
+    <tableColumn id="3" name="E-mail" dataDxfId="11"/>
+    <tableColumn id="4" name="CP" dataDxfId="10"/>
+    <tableColumn id="5" name="Tanggal Seleksi I" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:E51" totalsRowShown="0" headerRowDxfId="20" dataDxfId="19">
+  <autoFilter ref="A4:E51"/>
+  <sortState ref="A5:E51">
+    <sortCondition ref="B4:B51"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="1" name="NIM" dataDxfId="18"/>
+    <tableColumn id="2" name="Nama" dataDxfId="17"/>
+    <tableColumn id="3" name="E-mail" dataDxfId="16"/>
+    <tableColumn id="4" name="CP" dataDxfId="15"/>
+    <tableColumn id="5" name="Tanggal Seleksi I" dataDxfId="14"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A4:E26" totalsRowShown="0" headerRowDxfId="0" dataDxfId="1">
+  <autoFilter ref="A4:E26"/>
+  <sortState ref="A5:E26">
+    <sortCondition ref="B4:B26"/>
+  </sortState>
   <tableColumns count="5">
     <tableColumn id="1" name="NIM" dataDxfId="6"/>
     <tableColumn id="2" name="Nama" dataDxfId="5"/>
@@ -668,7 +1007,7 @@
   <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -676,7 +1015,7 @@
     <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
     <col min="2" max="2" width="35.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.85546875" style="10" customWidth="1"/>
     <col min="5" max="5" width="24.5703125" style="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -685,13 +1024,17 @@
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:5" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+        <v>37</v>
+      </c>
+      <c r="D2" s="9"/>
+    </row>
+    <row r="3" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D3" s="8"/>
+    </row>
     <row r="4" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
@@ -702,7 +1045,7 @@
       <c r="C4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="8" t="s">
         <v>4</v>
       </c>
       <c r="E4" s="2" t="s">
@@ -711,91 +1054,220 @@
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>8</v>
+        <v>10</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E6" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="9" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="10" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="11" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="12" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="14" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="15" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="16" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="17" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="18" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="19" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="21" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="22" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="23" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="24" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="25" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="26" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="27" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="28" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="29" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="30" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    </row>
+    <row r="7" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>50</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" s="11" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="8"/>
+    </row>
+    <row r="15" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="8"/>
+    </row>
+    <row r="16" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="8"/>
+    </row>
+    <row r="17" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="8"/>
+    </row>
+    <row r="18" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="8"/>
+    </row>
+    <row r="19" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="8"/>
+    </row>
+    <row r="20" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="8"/>
+    </row>
+    <row r="21" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="8"/>
+    </row>
+    <row r="22" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="8"/>
+    </row>
+    <row r="23" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="8"/>
+    </row>
+    <row r="24" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D24" s="8"/>
+    </row>
+    <row r="25" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D25" s="8"/>
+    </row>
+    <row r="26" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D26" s="8"/>
+    </row>
+    <row r="27" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D27" s="8"/>
+    </row>
+    <row r="28" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D28" s="8"/>
+    </row>
+    <row r="29" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D29" s="8"/>
+    </row>
+    <row r="30" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D30" s="8"/>
+    </row>
+    <row r="31" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D31" s="8"/>
+    </row>
+    <row r="32" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D32" s="8"/>
+    </row>
+    <row r="33" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D33" s="8"/>
+    </row>
+    <row r="34" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D34" s="8"/>
+    </row>
+    <row r="35" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D35" s="8"/>
+    </row>
+    <row r="36" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D36" s="8"/>
+    </row>
+    <row r="37" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D37" s="8"/>
+    </row>
+    <row r="38" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D38" s="8"/>
+    </row>
+    <row r="39" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D39" s="8"/>
+    </row>
+    <row r="40" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D40" s="8"/>
+    </row>
+    <row r="41" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D41" s="8"/>
+    </row>
+    <row r="42" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D42" s="8"/>
+    </row>
+    <row r="43" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D43" s="8"/>
+    </row>
+    <row r="44" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D44" s="8"/>
+    </row>
+    <row r="45" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D45" s="8"/>
+    </row>
+    <row r="46" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D46" s="8"/>
+    </row>
+    <row r="47" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D47" s="8"/>
+    </row>
+    <row r="48" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D48" s="8"/>
+    </row>
+    <row r="49" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D49" s="8"/>
+    </row>
+    <row r="50" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D50" s="8"/>
+    </row>
+    <row r="51" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D51" s="8"/>
+    </row>
+    <row r="52" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D52" s="8"/>
+    </row>
+    <row r="53" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D53" s="8"/>
+    </row>
+    <row r="54" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D54" s="8"/>
+    </row>
+    <row r="55" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D55" s="8"/>
+    </row>
+    <row r="56" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D56" s="8"/>
+    </row>
+    <row r="57" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D57" s="8"/>
+    </row>
+    <row r="58" spans="4:4" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D58" s="8"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1"/>
-    <hyperlink ref="C6" r:id="rId2"/>
+    <hyperlink ref="C8" r:id="rId1"/>
+    <hyperlink ref="C5" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId4"/>
+  </tableParts>
 </worksheet>
 </file>
 
@@ -803,8 +1275,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -824,7 +1296,7 @@
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -847,168 +1319,307 @@
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
+        <v>31</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="6" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
+        <v>23</v>
+      </c>
     </row>
     <row r="7" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B7" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
-        <v>15</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="2" t="s">
-        <v>16</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="2" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="2" t="s">
-        <v>18</v>
-      </c>
+      <c r="A11" s="6"/>
+      <c r="B11" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="6"/>
+      <c r="D11" s="6"/>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="2" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="2" t="s">
-        <v>20</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="2" t="s">
-        <v>21</v>
-      </c>
+      <c r="A14" s="6"/>
+      <c r="B14" s="6" t="s">
+        <v>44</v>
+      </c>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="2" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="2" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="17" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+      <c r="C16" s="3"/>
+      <c r="D16" s="4"/>
+    </row>
+    <row r="17" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="2" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E19" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="18" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="20" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
+    <row r="22" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B26" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B27" s="2" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C28" s="3"/>
+      <c r="D28" s="4"/>
+    </row>
+    <row r="29" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B29" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B31" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="22" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="23" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="24" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="25" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="26" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="27" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="28" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="29" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="2" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="30" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="31" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="32" spans="2:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="33" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="34" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="35" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="36" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="37" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="38" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="39" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="40" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="41" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="42" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="43" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="44" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="45" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="46" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="47" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="48" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="49" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="50" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="51" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="52" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="53" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="54" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="55" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="56" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="57" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="58" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="32" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="6"/>
+      <c r="C32" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+    </row>
+    <row r="33" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="6"/>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="6"/>
+    </row>
+    <row r="34" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="6"/>
+      <c r="B34" s="6"/>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="6"/>
+    </row>
+    <row r="35" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="6"/>
+      <c r="B35" s="6"/>
+      <c r="C35" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="6"/>
+    </row>
+    <row r="36" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="6"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+    </row>
+    <row r="37" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="6"/>
+      <c r="B37" s="6"/>
+      <c r="C37" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="6"/>
+    </row>
+    <row r="38" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="6"/>
+      <c r="B38" s="6"/>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+    </row>
+    <row r="39" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="6"/>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+    </row>
+    <row r="40" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="6"/>
+      <c r="B40" s="6"/>
+      <c r="C40" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="6"/>
+    </row>
+    <row r="41" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="6"/>
+      <c r="B41" s="6"/>
+      <c r="C41" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="6"/>
+    </row>
+    <row r="42" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="6"/>
+      <c r="B42" s="6"/>
+      <c r="C42" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="6"/>
+    </row>
+    <row r="43" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+    </row>
+    <row r="44" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="6"/>
+      <c r="B44" s="6"/>
+      <c r="C44" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="6"/>
+    </row>
+    <row r="45" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="6"/>
+      <c r="B45" s="6"/>
+      <c r="C45" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="6"/>
+    </row>
+    <row r="46" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="6"/>
+      <c r="B46" s="6"/>
+      <c r="C46" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="6"/>
+    </row>
+    <row r="47" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="6"/>
+      <c r="B47" s="6"/>
+      <c r="C47" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="6"/>
+    </row>
+    <row r="48" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="6"/>
+      <c r="B48" s="6"/>
+      <c r="C48" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="6"/>
+    </row>
+    <row r="49" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="6"/>
+      <c r="B49" s="6"/>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+    </row>
+    <row r="50" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="6"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+    </row>
+    <row r="51" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="6"/>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+    </row>
+    <row r="52" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="53" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="54" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="55" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="56" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="57" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="58" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
@@ -1021,8 +1632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1045,7 +1656,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -1078,7 +1689,7 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>40</v>
@@ -1089,10 +1700,10 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="4"/>
@@ -1261,5 +1872,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Edit pesertaseleksidb -> Tambah Peserta.
</commit_message>
<xml_diff>
--- a/pesertaseleksidb.xlsx
+++ b/pesertaseleksidb.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
   <si>
     <t>Daftar Peserta Seleksi Pengurus UKM - KMK Mikroskil Medan Periode 2015/2016</t>
   </si>
@@ -185,6 +185,60 @@
   </si>
   <si>
     <t>085261775689</t>
+  </si>
+  <si>
+    <t>14111-3473</t>
+  </si>
+  <si>
+    <t>Ami Aivya Sibarani</t>
+  </si>
+  <si>
+    <t>085297462566</t>
+  </si>
+  <si>
+    <t>14111-3619</t>
+  </si>
+  <si>
+    <t>Eben Roy H. Silalahi</t>
+  </si>
+  <si>
+    <t>082165152615</t>
+  </si>
+  <si>
+    <t>14811-1411</t>
+  </si>
+  <si>
+    <t>Dian Kristian Silaban</t>
+  </si>
+  <si>
+    <t>085206514334</t>
+  </si>
+  <si>
+    <t>14811-1497</t>
+  </si>
+  <si>
+    <t>Widia Marito Manulang</t>
+  </si>
+  <si>
+    <t>082276099679</t>
+  </si>
+  <si>
+    <t>14811-1705</t>
+  </si>
+  <si>
+    <t>Shinta Warni Meliala</t>
+  </si>
+  <si>
+    <t>085761761106</t>
+  </si>
+  <si>
+    <t>14811-0459</t>
+  </si>
+  <si>
+    <t>Yuliana Siahaan</t>
+  </si>
+  <si>
+    <t>085372781223</t>
   </si>
 </sst>
 </file>
@@ -192,7 +246,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -270,13 +324,13 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -309,7 +363,7 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+      <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -716,7 +770,7 @@
   <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -852,34 +906,88 @@
       </c>
     </row>
     <row r="11" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="9"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="6"/>
+      <c r="A11" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D11" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="6">
+        <v>42187</v>
+      </c>
     </row>
     <row r="12" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="9"/>
-      <c r="D12" s="9"/>
-      <c r="E12" s="6"/>
+      <c r="A12" s="9" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="D12" s="9" t="s">
+        <v>58</v>
+      </c>
+      <c r="E12" s="6">
+        <v>42187</v>
+      </c>
     </row>
     <row r="13" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="6"/>
+      <c r="A13" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="E13" s="6">
+        <v>42188</v>
+      </c>
     </row>
     <row r="14" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="9"/>
-      <c r="D14" s="9"/>
-      <c r="E14" s="6"/>
+      <c r="A14" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D14" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="E14" s="6">
+        <v>42188</v>
+      </c>
     </row>
     <row r="15" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="9"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="6"/>
+      <c r="A15" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="D15" s="9" t="s">
+        <v>67</v>
+      </c>
+      <c r="E15" s="6">
+        <v>42188</v>
+      </c>
     </row>
     <row r="16" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="9"/>
-      <c r="D16" s="9"/>
-      <c r="E16" s="6"/>
+      <c r="A16" s="9" t="s">
+        <v>68</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="D16" s="9" t="s">
+        <v>70</v>
+      </c>
+      <c r="E16" s="6">
+        <v>42188</v>
+      </c>
     </row>
     <row r="17" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
@@ -1108,7 +1216,7 @@
     <sheetView topLeftCell="A4" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="A4" sqref="A4"/>
-      <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Edit pesertaseleksidb.xlsx -> Tambah Peserta.
</commit_message>
<xml_diff>
--- a/pesertaseleksidb.xlsx
+++ b/pesertaseleksidb.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
   <si>
     <t>Daftar Peserta Seleksi Pengurus UKM - KMK Mikroskil Medan Periode 2015/2016</t>
   </si>
@@ -239,6 +239,15 @@
   </si>
   <si>
     <t>085372781223</t>
+  </si>
+  <si>
+    <t>Lihardo Rawaja Haloho</t>
+  </si>
+  <si>
+    <t>082276845356</t>
+  </si>
+  <si>
+    <t>haloholihardo@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -309,7 +318,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -339,6 +348,9 @@
     </xf>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -770,7 +782,7 @@
   <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -991,8 +1003,18 @@
     </row>
     <row r="17" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="9"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="6"/>
+      <c r="B17" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E17" s="6">
+        <v>42187</v>
+      </c>
     </row>
     <row r="18" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9"/>
@@ -1203,9 +1225,10 @@
   <hyperlinks>
     <hyperlink ref="C5" r:id="rId1"/>
     <hyperlink ref="C6" r:id="rId2"/>
+    <hyperlink ref="C17" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Edit 'pesertaseleksidb.xlsx' -> Tambah Peserta.
</commit_message>
<xml_diff>
--- a/pesertaseleksidb.xlsx
+++ b/pesertaseleksidb.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="99" uniqueCount="86">
   <si>
     <t>Daftar Peserta Seleksi Pengurus UKM - KMK Mikroskil Medan Periode 2015/2016</t>
   </si>
@@ -248,6 +248,42 @@
   </si>
   <si>
     <t>haloholihardo@gmail.com</t>
+  </si>
+  <si>
+    <t>14211-3061</t>
+  </si>
+  <si>
+    <t>Nita Febrina Butar-butar</t>
+  </si>
+  <si>
+    <t>087744750232</t>
+  </si>
+  <si>
+    <t>14211-3771</t>
+  </si>
+  <si>
+    <t>Sisilya Dewi Siregar</t>
+  </si>
+  <si>
+    <t>082276876382</t>
+  </si>
+  <si>
+    <t>13211-2964</t>
+  </si>
+  <si>
+    <t>Indah Priskila Butar-butar</t>
+  </si>
+  <si>
+    <t>081281128784</t>
+  </si>
+  <si>
+    <t>13211-2476</t>
+  </si>
+  <si>
+    <t>Imelda Sadna Sianturi</t>
+  </si>
+  <si>
+    <t>082370246730</t>
   </si>
 </sst>
 </file>
@@ -782,7 +818,7 @@
   <dimension ref="A1:E58"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1017,24 +1053,60 @@
       </c>
     </row>
     <row r="18" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="9"/>
-      <c r="D18" s="9"/>
-      <c r="E18" s="6"/>
+      <c r="A18" s="9" t="s">
+        <v>74</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="D18" s="9" t="s">
+        <v>76</v>
+      </c>
+      <c r="E18" s="6">
+        <v>42187</v>
+      </c>
     </row>
     <row r="19" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="9"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="6"/>
+      <c r="A19" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D19" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="E19" s="6">
+        <v>42188</v>
+      </c>
     </row>
     <row r="20" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="9"/>
-      <c r="D20" s="9"/>
-      <c r="E20" s="6"/>
+      <c r="A20" s="9" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20" s="9" t="s">
+        <v>82</v>
+      </c>
+      <c r="E20" s="6">
+        <v>42188</v>
+      </c>
     </row>
     <row r="21" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="9"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="6"/>
+      <c r="A21" s="9" t="s">
+        <v>83</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D21" s="9" t="s">
+        <v>85</v>
+      </c>
+      <c r="E21" s="6">
+        <v>42188</v>
+      </c>
     </row>
     <row r="22" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="9"/>

</xml_diff>

<commit_message>
Edit 'pesertaseleksidb.xlsx' -> Tambah Peserta; Edit Tampilan.
</commit_message>
<xml_diff>
--- a/pesertaseleksidb.xlsx
+++ b/pesertaseleksidb.xlsx
@@ -394,7 +394,112 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="13">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -536,17 +641,34 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:E29" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="A4:E1048576" totalsRowShown="0" dataDxfId="0">
+  <autoFilter ref="A4:E1048576"/>
+  <sortState ref="A5:E58">
+    <sortCondition ref="B4:B1048576"/>
+  </sortState>
+  <tableColumns count="5">
+    <tableColumn id="1" name="NIM" dataDxfId="5"/>
+    <tableColumn id="2" name="Nama" dataDxfId="4"/>
+    <tableColumn id="3" name="E-mail" dataDxfId="3"/>
+    <tableColumn id="4" name="CP" dataDxfId="2"/>
+    <tableColumn id="5" name="Tanggal Seleksi I" dataDxfId="1"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:E29" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11">
   <autoFilter ref="A4:E29"/>
   <sortState ref="A5:E29">
     <sortCondition ref="B4:B29"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="NIM" dataDxfId="4"/>
-    <tableColumn id="2" name="Nama" dataDxfId="3"/>
-    <tableColumn id="3" name="E-mail" dataDxfId="2"/>
-    <tableColumn id="4" name="CP" dataDxfId="1"/>
-    <tableColumn id="5" name="Tanggal Seleksi I" dataDxfId="0"/>
+    <tableColumn id="1" name="NIM" dataDxfId="10"/>
+    <tableColumn id="2" name="Nama" dataDxfId="9"/>
+    <tableColumn id="3" name="E-mail" dataDxfId="8"/>
+    <tableColumn id="4" name="CP" dataDxfId="7"/>
+    <tableColumn id="5" name="Tanggal Seleksi I" dataDxfId="6"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -817,8 +939,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -869,184 +993,184 @@
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="9" t="s">
-        <v>40</v>
+        <v>53</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>8</v>
-      </c>
-      <c r="E5" s="6"/>
+        <v>54</v>
+      </c>
+      <c r="D5" s="9" t="s">
+        <v>55</v>
+      </c>
+      <c r="E5" s="6">
+        <v>42187</v>
+      </c>
     </row>
     <row r="6" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="9" t="s">
-        <v>40</v>
+        <v>50</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D6" s="12" t="s">
-        <v>11</v>
-      </c>
-      <c r="E6" s="6"/>
+        <v>51</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="E6" s="6">
+        <v>42187</v>
+      </c>
     </row>
     <row r="7" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="9" t="s">
-        <v>44</v>
+        <v>59</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="D7" s="12" t="s">
-        <v>42</v>
+        <v>60</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>61</v>
       </c>
       <c r="E7" s="6">
-        <v>42187</v>
+        <v>42188</v>
       </c>
     </row>
     <row r="8" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="9" t="s">
-        <v>45</v>
+        <v>56</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>43</v>
+        <v>57</v>
       </c>
       <c r="D8" s="9" t="s">
-        <v>46</v>
+        <v>58</v>
       </c>
       <c r="E8" s="6">
-        <v>42189</v>
+        <v>42187</v>
       </c>
     </row>
     <row r="9" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9" t="s">
-        <v>47</v>
+        <v>83</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>48</v>
+        <v>84</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>49</v>
+        <v>85</v>
       </c>
       <c r="E9" s="6">
-        <v>42189</v>
+        <v>42188</v>
       </c>
     </row>
     <row r="10" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9" t="s">
-        <v>50</v>
+        <v>80</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>51</v>
+        <v>81</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>52</v>
+        <v>82</v>
       </c>
       <c r="E10" s="6">
-        <v>42187</v>
+        <v>42188</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="9" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D11" s="9" t="s">
-        <v>55</v>
-      </c>
-      <c r="E11" s="6">
-        <v>42187</v>
-      </c>
+        <v>9</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="9" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>57</v>
+        <v>43</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>58</v>
+        <v>46</v>
       </c>
       <c r="E12" s="6">
+        <v>42189</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="9"/>
+      <c r="B13" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>73</v>
+      </c>
+      <c r="D13" s="9" t="s">
+        <v>72</v>
+      </c>
+      <c r="E13" s="6">
         <v>42187</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>59</v>
-      </c>
-      <c r="B13" s="2" t="s">
-        <v>60</v>
-      </c>
-      <c r="D13" s="9" t="s">
-        <v>61</v>
-      </c>
-      <c r="E13" s="6">
-        <v>42188</v>
       </c>
     </row>
     <row r="14" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
-        <v>62</v>
+        <v>47</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>63</v>
+        <v>48</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="E14" s="6">
-        <v>42188</v>
+        <v>42189</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>67</v>
+        <v>76</v>
       </c>
       <c r="E15" s="6">
-        <v>42188</v>
+        <v>42187</v>
       </c>
     </row>
     <row r="16" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
-        <v>68</v>
+        <v>40</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>69</v>
-      </c>
-      <c r="D16" s="9" t="s">
-        <v>70</v>
-      </c>
-      <c r="E16" s="6">
-        <v>42188</v>
-      </c>
+        <v>6</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="E16" s="6"/>
     </row>
     <row r="17" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="9"/>
+      <c r="A17" s="9" t="s">
+        <v>44</v>
+      </c>
       <c r="B17" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C17" s="13" t="s">
-        <v>73</v>
-      </c>
-      <c r="D17" s="9" t="s">
-        <v>72</v>
+        <v>41</v>
+      </c>
+      <c r="D17" s="12" t="s">
+        <v>42</v>
       </c>
       <c r="E17" s="6">
         <v>42187</v>
@@ -1054,16 +1178,16 @@
     </row>
     <row r="18" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="E18" s="6">
-        <v>42187</v>
+        <v>42188</v>
       </c>
     </row>
     <row r="19" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1082,13 +1206,13 @@
     </row>
     <row r="20" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="9" t="s">
-        <v>80</v>
+        <v>62</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="E20" s="6">
         <v>42188</v>
@@ -1096,13 +1220,13 @@
     </row>
     <row r="21" spans="1:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="9" t="s">
-        <v>83</v>
+        <v>68</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>84</v>
+        <v>69</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>85</v>
+        <v>70</v>
       </c>
       <c r="E21" s="6">
         <v>42188</v>
@@ -1295,12 +1419,15 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="C5" r:id="rId1"/>
-    <hyperlink ref="C6" r:id="rId2"/>
-    <hyperlink ref="C17" r:id="rId3"/>
+    <hyperlink ref="C16" r:id="rId1"/>
+    <hyperlink ref="C11" r:id="rId2"/>
+    <hyperlink ref="C13" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
+  <tableParts count="1">
+    <tablePart r:id="rId5"/>
+  </tableParts>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
data 26 juni 2015, jam 13:30
</commit_message>
<xml_diff>
--- a/pesertaseleksidb.xlsx
+++ b/pesertaseleksidb.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="109">
   <si>
     <t>Daftar Peserta Seleksi Pengurus UKM - KMK Mikroskil Medan Periode 2015/2016</t>
   </si>
@@ -302,13 +302,64 @@
   </si>
   <si>
     <t>082276099679</t>
+  </si>
+  <si>
+    <t>Keterangan</t>
+  </si>
+  <si>
+    <t>Merah</t>
+  </si>
+  <si>
+    <t>Mahasiswa bersangkutan tidak ada lagi di Mikroskil</t>
+  </si>
+  <si>
+    <t>Natalya Uli Purba</t>
+  </si>
+  <si>
+    <t>082273350631</t>
+  </si>
+  <si>
+    <t>Juni Susanti Siregar</t>
+  </si>
+  <si>
+    <t>082272756482</t>
+  </si>
+  <si>
+    <t>Ines Lidwina Damanik</t>
+  </si>
+  <si>
+    <t>085760260603</t>
+  </si>
+  <si>
+    <t>Anaria Novitasari Sitio</t>
+  </si>
+  <si>
+    <t>081269576256</t>
+  </si>
+  <si>
+    <t>Surya Simarmata</t>
+  </si>
+  <si>
+    <t>085763552786</t>
+  </si>
+  <si>
+    <t>Johannes Putra Rezeki Sianturi</t>
+  </si>
+  <si>
+    <t>081265361098</t>
+  </si>
+  <si>
+    <t>Kevin Julianto Alexander Pane</t>
+  </si>
+  <si>
+    <t>081262958404</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -353,13 +404,26 @@
       <name val="Calibri"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF68686"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -375,7 +439,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -418,12 +482,81 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="27">
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -860,6 +993,13 @@
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF68686"/>
+      <color rgb="FFF35757"/>
+      <color rgb="FFFF3737"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -872,50 +1012,60 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:F29" totalsRowShown="0" headerRowDxfId="23" dataDxfId="22">
-  <autoFilter ref="B4:F29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:F33" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+  <autoFilter ref="B4:F33"/>
   <sortState ref="B5:F29">
     <sortCondition ref="C4:C29"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="NIM" dataDxfId="21"/>
-    <tableColumn id="2" name="Nama" dataDxfId="20"/>
-    <tableColumn id="3" name="E-mail" dataDxfId="19"/>
-    <tableColumn id="4" name="CP" dataDxfId="18"/>
-    <tableColumn id="5" name="Tanggal Seleksi I" dataDxfId="17"/>
+    <tableColumn id="1" name="NIM" dataDxfId="24"/>
+    <tableColumn id="2" name="Nama" dataDxfId="23"/>
+    <tableColumn id="3" name="E-mail" dataDxfId="22"/>
+    <tableColumn id="4" name="CP" dataDxfId="21"/>
+    <tableColumn id="5" name="Tanggal Seleksi I" dataDxfId="20"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A4:A29" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
-  <autoFilter ref="A4:A29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A4:A33" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A4:A33"/>
   <tableColumns count="1">
-    <tableColumn id="1" name="No" dataDxfId="14"/>
+    <tableColumn id="1" name="No" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A4:E51" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12">
-  <autoFilter ref="A4:E51"/>
-  <sortState ref="A5:E51">
-    <sortCondition ref="B4:B51"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="B4:F51" totalsRowShown="0" headerRowDxfId="16" dataDxfId="15">
+  <autoFilter ref="B4:F51"/>
+  <sortState ref="B5:F51">
+    <sortCondition ref="C4:C51"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="NIM" dataDxfId="11"/>
-    <tableColumn id="2" name="Nama" dataDxfId="10"/>
-    <tableColumn id="3" name="E-mail" dataDxfId="9"/>
-    <tableColumn id="4" name="CP" dataDxfId="8"/>
-    <tableColumn id="5" name="Tanggal Seleksi I" dataDxfId="7"/>
+    <tableColumn id="1" name="NIM" dataDxfId="14"/>
+    <tableColumn id="2" name="Nama" dataDxfId="13"/>
+    <tableColumn id="3" name="E-mail" dataDxfId="12"/>
+    <tableColumn id="4" name="CP" dataDxfId="11"/>
+    <tableColumn id="5" name="Tanggal Seleksi I" dataDxfId="10"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="6" name="Table6" displayName="Table6" ref="A4:A51" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A4:A51"/>
+  <tableColumns count="1">
+    <tableColumn id="1" name="No" dataDxfId="7"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A4:E26" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
   <autoFilter ref="A4:E26"/>
   <sortState ref="A5:E26">
@@ -1197,8 +1347,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1251,31 +1401,31 @@
       <c r="A5" s="2">
         <v>1</v>
       </c>
-      <c r="B5" s="2" t="s">
-        <v>41</v>
+      <c r="B5" s="2">
+        <v>141113473</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="11" t="s">
-        <v>11</v>
+        <v>77</v>
+      </c>
+      <c r="E5" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>2</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>47</v>
+      <c r="B6" s="2">
+        <v>141110841</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>49</v>
+        <v>69</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
       <c r="F6" s="2" t="s">
         <v>42</v>
@@ -1285,14 +1435,14 @@
       <c r="A7" s="2">
         <v>3</v>
       </c>
-      <c r="B7" s="2" t="s">
-        <v>47</v>
+      <c r="B7" s="2">
+        <v>141112974</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>50</v>
+        <v>65</v>
+      </c>
+      <c r="E7" s="8" t="s">
+        <v>66</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>42</v>
@@ -1303,33 +1453,33 @@
         <v>4</v>
       </c>
       <c r="B8" s="2">
-        <v>142113061</v>
+        <v>148111411</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>53</v>
+        <v>88</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>54</v>
+        <v>89</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>55</v>
+        <v>43</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>5</v>
       </c>
-      <c r="B9" s="2" t="s">
-        <v>41</v>
+      <c r="B9" s="2">
+        <v>141114380</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="E9" s="11" t="s">
-        <v>8</v>
+        <v>75</v>
+      </c>
+      <c r="E9" s="8" t="s">
+        <v>76</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1337,16 +1487,16 @@
         <v>6</v>
       </c>
       <c r="B10" s="2">
-        <v>142113771</v>
+        <v>141110736</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>56</v>
+        <v>67</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>57</v>
+        <v>68</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1354,13 +1504,13 @@
         <v>7</v>
       </c>
       <c r="B11" s="2">
-        <v>132112964</v>
+        <v>132112476</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F11" s="2" t="s">
         <v>43</v>
@@ -1371,13 +1521,13 @@
         <v>8</v>
       </c>
       <c r="B12" s="2">
-        <v>132112476</v>
+        <v>132112964</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F12" s="2" t="s">
         <v>43</v>
@@ -1387,17 +1537,17 @@
       <c r="A13" s="2">
         <v>9</v>
       </c>
-      <c r="B13" s="2">
-        <v>141112974</v>
+      <c r="B13" s="2" t="s">
+        <v>41</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>65</v>
-      </c>
-      <c r="E13" s="8" t="s">
-        <v>66</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>42</v>
+        <v>9</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1405,30 +1555,30 @@
         <v>10</v>
       </c>
       <c r="B14" s="2">
-        <v>141110736</v>
+        <v>148111136</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>67</v>
+        <v>97</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>68</v>
+        <v>98</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>11</v>
       </c>
-      <c r="B15" s="2">
-        <v>141110841</v>
+      <c r="B15" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>70</v>
+        <v>51</v>
       </c>
       <c r="F15" s="2" t="s">
         <v>42</v>
@@ -1438,31 +1588,31 @@
       <c r="A16" s="2">
         <v>12</v>
       </c>
-      <c r="B16" s="2">
-        <v>141114509</v>
-      </c>
       <c r="C16" s="2" t="s">
-        <v>71</v>
+        <v>79</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>80</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>13</v>
       </c>
-      <c r="B17" s="2">
-        <v>141114584</v>
+      <c r="B17" s="2" t="s">
+        <v>47</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E17" s="8" t="s">
-        <v>74</v>
+        <v>48</v>
+      </c>
+      <c r="E17" s="12" t="s">
+        <v>50</v>
       </c>
       <c r="F17" s="2" t="s">
         <v>42</v>
@@ -1473,16 +1623,16 @@
         <v>14</v>
       </c>
       <c r="B18" s="2">
-        <v>141114380</v>
+        <v>141113881</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>75</v>
+        <v>95</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>76</v>
+        <v>96</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1490,33 +1640,33 @@
         <v>15</v>
       </c>
       <c r="B19" s="2">
-        <v>141113473</v>
+        <v>142113061</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>77</v>
+        <v>53</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>78</v>
+        <v>54</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>42</v>
+        <v>55</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>16</v>
       </c>
+      <c r="B20" s="2" t="s">
+        <v>41</v>
+      </c>
       <c r="C20" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="D20" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>81</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>55</v>
+        <v>6</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E20" s="11" t="s">
+        <v>8</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1524,16 +1674,16 @@
         <v>17</v>
       </c>
       <c r="B21" s="2">
-        <v>141112583</v>
+        <v>141114509</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1541,16 +1691,16 @@
         <v>18</v>
       </c>
       <c r="B22" s="2">
-        <v>148110459</v>
+        <v>141112583</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1575,16 +1725,16 @@
         <v>20</v>
       </c>
       <c r="B24" s="2">
-        <v>148111411</v>
+        <v>142113771</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>88</v>
+        <v>56</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>89</v>
+        <v>57</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>43</v>
+        <v>55</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1592,97 +1742,193 @@
         <v>21</v>
       </c>
       <c r="B25" s="2">
-        <v>148111497</v>
+        <v>141114584</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>91</v>
+        <v>74</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>22</v>
       </c>
-      <c r="E26" s="8"/>
+      <c r="B26" s="2">
+        <v>148111497</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E26" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="27" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>23</v>
       </c>
-      <c r="E27" s="8"/>
+      <c r="B27" s="2">
+        <v>148110459</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="E27" s="8" t="s">
+        <v>85</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="28" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>24</v>
       </c>
-      <c r="E28" s="8"/>
+      <c r="B28" s="2">
+        <v>132113498</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="E28" s="8" t="s">
+        <v>100</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="29" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>25</v>
       </c>
-      <c r="E29" s="8"/>
+      <c r="B29" s="2">
+        <v>132112018</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="E29" s="8" t="s">
+        <v>102</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>42</v>
+      </c>
     </row>
     <row r="30" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E30" s="8"/>
+      <c r="A30" s="2">
+        <v>26</v>
+      </c>
+      <c r="B30" s="6">
+        <v>132112859</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>103</v>
+      </c>
+      <c r="D30" s="6"/>
+      <c r="E30" s="14" t="s">
+        <v>104</v>
+      </c>
+      <c r="F30" s="6" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="31" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E31" s="8"/>
+      <c r="A31" s="2">
+        <v>27</v>
+      </c>
+      <c r="B31" s="6">
+        <v>132112808</v>
+      </c>
+      <c r="C31" s="6" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" s="6"/>
+      <c r="E31" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="F31" s="6" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="32" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E32" s="8"/>
-    </row>
-    <row r="33" spans="5:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E33" s="8"/>
-    </row>
-    <row r="34" spans="5:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>28</v>
+      </c>
+      <c r="B32" s="6">
+        <v>132111101</v>
+      </c>
+      <c r="C32" s="6" t="s">
+        <v>107</v>
+      </c>
+      <c r="D32" s="6"/>
+      <c r="E32" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F32" s="6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>29</v>
+      </c>
+      <c r="B33" s="6"/>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="6"/>
+    </row>
+    <row r="34" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E34" s="8"/>
     </row>
-    <row r="35" spans="5:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E35" s="8"/>
     </row>
-    <row r="36" spans="5:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E36" s="8"/>
     </row>
-    <row r="37" spans="5:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E37" s="8"/>
     </row>
-    <row r="38" spans="5:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E38" s="8"/>
     </row>
-    <row r="39" spans="5:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E39" s="8"/>
     </row>
-    <row r="40" spans="5:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E40" s="8"/>
     </row>
-    <row r="41" spans="5:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E41" s="8"/>
     </row>
-    <row r="42" spans="5:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E42" s="8"/>
     </row>
-    <row r="43" spans="5:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E43" s="8"/>
     </row>
-    <row r="44" spans="5:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E44" s="8"/>
     </row>
-    <row r="45" spans="5:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E45" s="8"/>
     </row>
-    <row r="46" spans="5:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E46" s="8"/>
     </row>
-    <row r="47" spans="5:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E47" s="8"/>
     </row>
-    <row r="48" spans="5:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E48" s="8"/>
     </row>
     <row r="49" spans="5:5" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1717,9 +1963,9 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D9" r:id="rId1"/>
-    <hyperlink ref="D5" r:id="rId2"/>
-    <hyperlink ref="D20" r:id="rId3"/>
+    <hyperlink ref="D20" r:id="rId1"/>
+    <hyperlink ref="D13" r:id="rId2"/>
+    <hyperlink ref="D16" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId4"/>
@@ -1732,413 +1978,590 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E58"/>
+  <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H6" sqref="H6:K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
-    <col min="4" max="4" width="22.85546875" style="10" customWidth="1"/>
-    <col min="5" max="5" width="24.5703125" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="14.28515625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="35.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="27.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="22.85546875" style="10" customWidth="1"/>
+    <col min="6" max="6" width="24.5703125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="9.140625" style="1"/>
+    <col min="8" max="8" width="9.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="8"/>
-    </row>
-    <row r="2" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="E1" s="8"/>
+    </row>
+    <row r="2" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B2" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="D2" s="8"/>
-    </row>
-    <row r="3" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D3" s="8"/>
-    </row>
-    <row r="4" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="D4" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="8" t="s">
+      <c r="E4" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
+    <row r="5" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>1</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="D5" s="8"/>
-      <c r="E5" s="2" t="s">
+      <c r="E5" s="8"/>
+      <c r="F5" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="6" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="2" t="s">
+    <row r="6" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>2</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="8"/>
-    </row>
-    <row r="7" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
+      <c r="E6" s="8"/>
+      <c r="H6" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" s="18"/>
+      <c r="J6" s="18"/>
+      <c r="K6" s="18"/>
+    </row>
+    <row r="7" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>3</v>
+      </c>
+      <c r="C7" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="8"/>
-    </row>
-    <row r="8" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B8" s="2" t="s">
+      <c r="E7" s="8"/>
+      <c r="H7" s="19" t="s">
+        <v>93</v>
+      </c>
+      <c r="I7" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="J7" s="20"/>
+      <c r="K7" s="20"/>
+    </row>
+    <row r="8" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>4</v>
+      </c>
+      <c r="C8" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="D8" s="8"/>
-    </row>
-    <row r="9" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="2" t="s">
+      <c r="E8" s="8"/>
+      <c r="H8" s="19"/>
+      <c r="I8" s="20"/>
+      <c r="J8" s="20"/>
+      <c r="K8" s="20"/>
+    </row>
+    <row r="9" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>5</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="D9" s="8"/>
-    </row>
-    <row r="10" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2">
         <v>141113759</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="D10" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="D10" s="8" t="s">
+      <c r="E10" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="E10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="11" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
-      <c r="B11" s="6" t="s">
+    <row r="11" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>7</v>
+      </c>
+      <c r="B11" s="6"/>
+      <c r="C11" s="6" t="s">
         <v>46</v>
       </c>
-      <c r="C11" s="6"/>
-      <c r="D11" s="14"/>
-      <c r="E11" s="6"/>
-    </row>
-    <row r="12" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="2" t="s">
+      <c r="D11" s="6"/>
+      <c r="E11" s="14"/>
+      <c r="F11" s="6"/>
+    </row>
+    <row r="12" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>8</v>
+      </c>
+      <c r="C12" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="8"/>
-    </row>
-    <row r="13" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="2" t="s">
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="D13" s="8"/>
-    </row>
-    <row r="14" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
-      <c r="B14" s="6" t="s">
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>10</v>
+      </c>
+      <c r="B14" s="6"/>
+      <c r="C14" s="6" t="s">
         <v>44</v>
       </c>
-      <c r="C14" s="6"/>
-      <c r="D14" s="14"/>
-      <c r="E14" s="6"/>
-    </row>
-    <row r="15" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="2" t="s">
+      <c r="D14" s="6"/>
+      <c r="E14" s="14"/>
+      <c r="F14" s="6"/>
+    </row>
+    <row r="15" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>11</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="8"/>
-    </row>
-    <row r="16" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="2" t="s">
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>12</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="3"/>
-      <c r="D16" s="15"/>
-    </row>
-    <row r="17" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="2" t="s">
+      <c r="D16" s="3"/>
+      <c r="E16" s="15"/>
+    </row>
+    <row r="17" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>13</v>
+      </c>
+      <c r="C17" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="8"/>
-    </row>
-    <row r="18" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="2" t="s">
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="16">
+        <v>14</v>
+      </c>
+      <c r="B18" s="16"/>
+      <c r="C18" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="D18" s="8"/>
-    </row>
-    <row r="19" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B19" s="2" t="s">
+      <c r="D18" s="16"/>
+      <c r="E18" s="17"/>
+      <c r="F18" s="16"/>
+    </row>
+    <row r="19" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>15</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="D19" s="8"/>
-      <c r="E19" s="7" t="s">
+      <c r="E19" s="8"/>
+      <c r="F19" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="2" t="s">
+    <row r="20" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="16">
+        <v>16</v>
+      </c>
+      <c r="B20" s="16"/>
+      <c r="C20" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="8"/>
-    </row>
-    <row r="21" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="2" t="s">
+      <c r="D20" s="16"/>
+      <c r="E20" s="17"/>
+      <c r="F20" s="16"/>
+    </row>
+    <row r="21" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>17</v>
+      </c>
+      <c r="C21" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="D21" s="8"/>
-    </row>
-    <row r="22" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B22" s="2" t="s">
+      <c r="E21" s="8"/>
+    </row>
+    <row r="22" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>18</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="D22" s="8"/>
-    </row>
-    <row r="23" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B23" s="2" t="s">
+      <c r="E22" s="8"/>
+    </row>
+    <row r="23" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>19</v>
+      </c>
+      <c r="C23" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="D23" s="8"/>
-    </row>
-    <row r="24" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="2" t="s">
+      <c r="E23" s="8"/>
+    </row>
+    <row r="24" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>20</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="D24" s="8"/>
-    </row>
-    <row r="25" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B25" s="2" t="s">
+      <c r="E24" s="8"/>
+    </row>
+    <row r="25" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>21</v>
+      </c>
+      <c r="C25" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="D25" s="8"/>
-    </row>
-    <row r="26" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B26" s="2" t="s">
+      <c r="E25" s="8"/>
+    </row>
+    <row r="26" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>22</v>
+      </c>
+      <c r="C26" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="D26" s="8"/>
-    </row>
-    <row r="27" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="2" t="s">
+      <c r="E26" s="8"/>
+    </row>
+    <row r="27" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>23</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="D27" s="8"/>
-    </row>
-    <row r="28" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="2" t="s">
+      <c r="E27" s="8"/>
+    </row>
+    <row r="28" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>24</v>
+      </c>
+      <c r="C28" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C28" s="3"/>
-      <c r="D28" s="15"/>
-    </row>
-    <row r="29" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="2" t="s">
+      <c r="D28" s="3"/>
+      <c r="E28" s="15"/>
+    </row>
+    <row r="29" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>25</v>
+      </c>
+      <c r="C29" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="D29" s="8"/>
-    </row>
-    <row r="30" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="2" t="s">
+      <c r="E29" s="8"/>
+    </row>
+    <row r="30" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>26</v>
+      </c>
+      <c r="C30" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="D30" s="8"/>
-      <c r="E30" s="2" t="s">
+      <c r="E30" s="8"/>
+      <c r="F30" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="31" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B31" s="2" t="s">
+    <row r="31" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
         <v>27</v>
       </c>
-      <c r="D31" s="8"/>
-    </row>
-    <row r="32" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
+      <c r="C31" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="E31" s="8"/>
+    </row>
+    <row r="32" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>28</v>
+      </c>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
-      <c r="D32" s="14"/>
-      <c r="E32" s="6"/>
-    </row>
-    <row r="33" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="6"/>
+    </row>
+    <row r="33" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>29</v>
+      </c>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
-      <c r="D33" s="14"/>
-      <c r="E33" s="6"/>
-    </row>
-    <row r="34" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
+      <c r="D33" s="6"/>
+      <c r="E33" s="14"/>
+      <c r="F33" s="6"/>
+    </row>
+    <row r="34" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>30</v>
+      </c>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="6"/>
-    </row>
-    <row r="35" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
+      <c r="D34" s="6"/>
+      <c r="E34" s="14"/>
+      <c r="F34" s="6"/>
+    </row>
+    <row r="35" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>31</v>
+      </c>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
-      <c r="D35" s="14"/>
-      <c r="E35" s="6"/>
-    </row>
-    <row r="36" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
+      <c r="D35" s="6"/>
+      <c r="E35" s="14"/>
+      <c r="F35" s="6"/>
+    </row>
+    <row r="36" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>32</v>
+      </c>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
-      <c r="D36" s="14"/>
-      <c r="E36" s="6"/>
-    </row>
-    <row r="37" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="14"/>
+      <c r="F36" s="6"/>
+    </row>
+    <row r="37" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>33</v>
+      </c>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
-      <c r="D37" s="14"/>
-      <c r="E37" s="6"/>
-    </row>
-    <row r="38" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
+      <c r="D37" s="6"/>
+      <c r="E37" s="14"/>
+      <c r="F37" s="6"/>
+    </row>
+    <row r="38" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>34</v>
+      </c>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
-      <c r="D38" s="14"/>
-      <c r="E38" s="6"/>
-    </row>
-    <row r="39" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="14"/>
+      <c r="F38" s="6"/>
+    </row>
+    <row r="39" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>35</v>
+      </c>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
-      <c r="D39" s="14"/>
-      <c r="E39" s="6"/>
-    </row>
-    <row r="40" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
+      <c r="D39" s="6"/>
+      <c r="E39" s="14"/>
+      <c r="F39" s="6"/>
+    </row>
+    <row r="40" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>36</v>
+      </c>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
-      <c r="D40" s="14"/>
-      <c r="E40" s="6"/>
-    </row>
-    <row r="41" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
+      <c r="D40" s="6"/>
+      <c r="E40" s="14"/>
+      <c r="F40" s="6"/>
+    </row>
+    <row r="41" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>37</v>
+      </c>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
-      <c r="D41" s="14"/>
-      <c r="E41" s="6"/>
-    </row>
-    <row r="42" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
+      <c r="D41" s="6"/>
+      <c r="E41" s="14"/>
+      <c r="F41" s="6"/>
+    </row>
+    <row r="42" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>38</v>
+      </c>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
-      <c r="D42" s="14"/>
-      <c r="E42" s="6"/>
-    </row>
-    <row r="43" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
+      <c r="D42" s="6"/>
+      <c r="E42" s="14"/>
+      <c r="F42" s="6"/>
+    </row>
+    <row r="43" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>39</v>
+      </c>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
-      <c r="D43" s="14"/>
-      <c r="E43" s="6"/>
-    </row>
-    <row r="44" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="14"/>
+      <c r="F43" s="6"/>
+    </row>
+    <row r="44" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>40</v>
+      </c>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
-      <c r="D44" s="14"/>
-      <c r="E44" s="6"/>
-    </row>
-    <row r="45" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
+      <c r="D44" s="6"/>
+      <c r="E44" s="14"/>
+      <c r="F44" s="6"/>
+    </row>
+    <row r="45" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>41</v>
+      </c>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
-      <c r="D45" s="14"/>
-      <c r="E45" s="6"/>
-    </row>
-    <row r="46" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
+      <c r="D45" s="6"/>
+      <c r="E45" s="14"/>
+      <c r="F45" s="6"/>
+    </row>
+    <row r="46" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>42</v>
+      </c>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
-      <c r="D46" s="14"/>
-      <c r="E46" s="6"/>
-    </row>
-    <row r="47" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
+      <c r="D46" s="6"/>
+      <c r="E46" s="14"/>
+      <c r="F46" s="6"/>
+    </row>
+    <row r="47" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>43</v>
+      </c>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
-      <c r="D47" s="14"/>
-      <c r="E47" s="6"/>
-    </row>
-    <row r="48" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
+      <c r="D47" s="6"/>
+      <c r="E47" s="14"/>
+      <c r="F47" s="6"/>
+    </row>
+    <row r="48" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>44</v>
+      </c>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
-      <c r="D48" s="14"/>
-      <c r="E48" s="6"/>
-    </row>
-    <row r="49" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
+      <c r="D48" s="6"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="6"/>
+    </row>
+    <row r="49" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>45</v>
+      </c>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
-      <c r="D49" s="14"/>
-      <c r="E49" s="6"/>
-    </row>
-    <row r="50" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="14"/>
+      <c r="F49" s="6"/>
+    </row>
+    <row r="50" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>46</v>
+      </c>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="6"/>
-    </row>
-    <row r="51" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="14"/>
+      <c r="F50" s="6"/>
+    </row>
+    <row r="51" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>47</v>
+      </c>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
-      <c r="D51" s="14"/>
-      <c r="E51" s="6"/>
-    </row>
-    <row r="52" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D52" s="8"/>
-    </row>
-    <row r="53" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D53" s="8"/>
-    </row>
-    <row r="54" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D54" s="8"/>
-    </row>
-    <row r="55" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D55" s="8"/>
-    </row>
-    <row r="56" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D56" s="8"/>
-    </row>
-    <row r="57" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D57" s="8"/>
-    </row>
-    <row r="58" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D58" s="8"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="14"/>
+      <c r="F51" s="6"/>
+    </row>
+    <row r="52" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E52" s="8"/>
+    </row>
+    <row r="53" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E53" s="8"/>
+    </row>
+    <row r="54" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E54" s="8"/>
+    </row>
+    <row r="55" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E55" s="8"/>
+    </row>
+    <row r="56" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E56" s="8"/>
+    </row>
+    <row r="57" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E57" s="8"/>
+    </row>
+    <row r="58" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E58" s="8"/>
     </row>
   </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="H6:K6"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:K8"/>
+  </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C10" r:id="rId1"/>
+    <hyperlink ref="D10" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId2"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
@@ -2148,7 +2571,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Edit pesertaseleksidb.xlsx -> Edit Tampilan.
</commit_message>
<xml_diff>
--- a/pesertaseleksidb.xlsx
+++ b/pesertaseleksidb.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2. Janward Alfredo Situmorang\KMK\KMK 2015\panitiaseleksikmk2015\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\mikroskil\kmkmikroskil\2015\pansel\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9195" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="MENDAFTAR" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="91">
   <si>
     <t>Daftar Peserta Seleksi Pengurus UKM - KMK Mikroskil Medan Periode 2015/2016</t>
   </si>
@@ -145,12 +145,6 @@
     <t>DIUNDANG</t>
   </si>
   <si>
-    <t>Eben Roy Silalahi</t>
-  </si>
-  <si>
-    <t>Derly Matondang</t>
-  </si>
-  <si>
     <t>TI (2014)</t>
   </si>
   <si>
@@ -302,6 +296,9 @@
   </si>
   <si>
     <t>082276099679</t>
+  </si>
+  <si>
+    <t>14111-3759</t>
   </si>
 </sst>
 </file>
@@ -440,6 +437,26 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
+      <numFmt numFmtId="30" formatCode="@"/>
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -566,25 +583,6 @@
         <name val="Calibri"/>
         <scheme val="minor"/>
       </font>
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="10"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <scheme val="minor"/>
-      </font>
-      <numFmt numFmtId="30" formatCode="@"/>
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -905,28 +903,28 @@
     <sortCondition ref="B4:B51"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="NIM" dataDxfId="11"/>
-    <tableColumn id="2" name="Nama" dataDxfId="10"/>
-    <tableColumn id="3" name="E-mail" dataDxfId="9"/>
-    <tableColumn id="4" name="CP" dataDxfId="8"/>
-    <tableColumn id="5" name="Tanggal Seleksi I" dataDxfId="7"/>
+    <tableColumn id="1" name="NIM" dataDxfId="1"/>
+    <tableColumn id="2" name="Nama" dataDxfId="11"/>
+    <tableColumn id="3" name="E-mail" dataDxfId="10"/>
+    <tableColumn id="4" name="CP" dataDxfId="0"/>
+    <tableColumn id="5" name="Tanggal Seleksi I" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A4:E26" totalsRowShown="0" headerRowDxfId="6" dataDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="3" name="Table3" displayName="Table3" ref="A4:E26" totalsRowShown="0" headerRowDxfId="8" dataDxfId="7">
   <autoFilter ref="A4:E26"/>
   <sortState ref="A5:E26">
     <sortCondition ref="B4:B26"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name="NIM" dataDxfId="4"/>
-    <tableColumn id="2" name="Nama" dataDxfId="3"/>
-    <tableColumn id="3" name="E-mail" dataDxfId="2"/>
-    <tableColumn id="4" name="CP" dataDxfId="1"/>
-    <tableColumn id="5" name="Tanggal Seleksi I" dataDxfId="0"/>
+    <tableColumn id="1" name="NIM" dataDxfId="6"/>
+    <tableColumn id="2" name="Nama" dataDxfId="5"/>
+    <tableColumn id="3" name="E-mail" dataDxfId="4"/>
+    <tableColumn id="4" name="CP" dataDxfId="3"/>
+    <tableColumn id="5" name="Tanggal Seleksi I" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1197,13 +1195,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView topLeftCell="A9" workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="1" max="1" width="4.42578125" style="1" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="35.42578125" style="1" customWidth="1"/>
     <col min="4" max="4" width="27.7109375" style="1" customWidth="1"/>
@@ -1229,7 +1227,7 @@
     </row>
     <row r="4" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
@@ -1252,7 +1250,7 @@
         <v>1</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C5" s="2" t="s">
         <v>9</v>
@@ -1269,16 +1267,16 @@
         <v>2</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="E6" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E6" s="8" t="s">
-        <v>51</v>
-      </c>
       <c r="F6" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1286,16 +1284,16 @@
         <v>3</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C7" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="12" t="s">
-        <v>50</v>
-      </c>
       <c r="F7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1306,13 +1304,13 @@
         <v>142113061</v>
       </c>
       <c r="C8" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="E8" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1320,7 +1318,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C9" s="2" t="s">
         <v>6</v>
@@ -1340,13 +1338,13 @@
         <v>142113771</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1357,13 +1355,13 @@
         <v>132112964</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1374,13 +1372,13 @@
         <v>132112476</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1391,13 +1389,13 @@
         <v>141112974</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1408,13 +1406,13 @@
         <v>141110736</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1425,13 +1423,13 @@
         <v>141110841</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E15" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F15" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1442,13 +1440,13 @@
         <v>141114509</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E16" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1459,13 +1457,13 @@
         <v>141114584</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1476,13 +1474,13 @@
         <v>141114380</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E18" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F18" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1493,13 +1491,13 @@
         <v>141113473</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E19" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1507,16 +1505,16 @@
         <v>16</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>81</v>
-      </c>
       <c r="F20" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1527,13 +1525,13 @@
         <v>141112583</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E21" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1544,13 +1542,13 @@
         <v>148110459</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1561,13 +1559,13 @@
         <v>148111705</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1578,13 +1576,13 @@
         <v>148111411</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E24" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F24" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1595,13 +1593,13 @@
         <v>148111497</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1734,13 +1732,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+    <sheetView topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.28515625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5703125" style="10" customWidth="1"/>
     <col min="2" max="2" width="35.42578125" style="1" customWidth="1"/>
     <col min="3" max="3" width="27.7109375" style="1" customWidth="1"/>
     <col min="4" max="4" width="22.85546875" style="10" customWidth="1"/>
@@ -1749,22 +1747,23 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="8"/>
     </row>
     <row r="2" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="9" t="s">
         <v>36</v>
       </c>
       <c r="D2" s="8"/>
     </row>
     <row r="3" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="8"/>
       <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="8" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1781,92 +1780,101 @@
       </c>
     </row>
     <row r="5" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="8"/>
       <c r="B5" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D5" s="8"/>
       <c r="E5" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
       <c r="B6" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D6" s="8"/>
     </row>
     <row r="7" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="8"/>
       <c r="B7" s="2" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="8"/>
     </row>
     <row r="8" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="8"/>
       <c r="B8" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D8" s="8"/>
     </row>
     <row r="9" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
       <c r="B9" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D9" s="8"/>
     </row>
     <row r="10" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>141113759</v>
+      <c r="A10" s="8" t="s">
+        <v>90</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>25</v>
       </c>
       <c r="C10" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D10" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="6"/>
+      <c r="A11" s="14"/>
       <c r="B11" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C11" s="6"/>
       <c r="D11" s="14"/>
       <c r="E11" s="6"/>
     </row>
     <row r="12" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A12" s="8"/>
       <c r="B12" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="8"/>
     </row>
     <row r="13" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
       <c r="B13" s="2" t="s">
         <v>26</v>
       </c>
       <c r="D13" s="8"/>
     </row>
     <row r="14" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="6"/>
+      <c r="A14" s="14"/>
       <c r="B14" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="14"/>
       <c r="E14" s="6"/>
     </row>
     <row r="15" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="8"/>
       <c r="B15" s="2" t="s">
         <v>14</v>
       </c>
       <c r="D15" s="8"/>
     </row>
     <row r="16" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="8"/>
       <c r="B16" s="2" t="s">
         <v>13</v>
       </c>
@@ -1874,75 +1882,87 @@
       <c r="D16" s="15"/>
     </row>
     <row r="17" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A17" s="8"/>
       <c r="B17" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D17" s="8"/>
     </row>
     <row r="18" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A18" s="8"/>
       <c r="B18" s="2" t="s">
         <v>34</v>
       </c>
       <c r="D18" s="8"/>
     </row>
     <row r="19" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="8"/>
       <c r="B19" s="2" t="s">
         <v>35</v>
       </c>
       <c r="D19" s="8"/>
       <c r="E19" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="8"/>
       <c r="B20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D20" s="8"/>
     </row>
     <row r="21" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="8"/>
       <c r="B21" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D21" s="8"/>
     </row>
     <row r="22" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A22" s="8"/>
       <c r="B22" s="2" t="s">
         <v>20</v>
       </c>
       <c r="D22" s="8"/>
     </row>
     <row r="23" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8"/>
       <c r="B23" s="2" t="s">
         <v>22</v>
       </c>
       <c r="D23" s="8"/>
     </row>
     <row r="24" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8"/>
       <c r="B24" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D24" s="8"/>
     </row>
     <row r="25" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="8"/>
       <c r="B25" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D25" s="8"/>
     </row>
     <row r="26" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8"/>
       <c r="B26" s="2" t="s">
         <v>30</v>
       </c>
       <c r="D26" s="8"/>
     </row>
     <row r="27" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8"/>
       <c r="B27" s="2" t="s">
         <v>33</v>
       </c>
       <c r="D27" s="8"/>
     </row>
     <row r="28" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="8"/>
       <c r="B28" s="2" t="s">
         <v>12</v>
       </c>
@@ -1950,185 +1970,195 @@
       <c r="D28" s="15"/>
     </row>
     <row r="29" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8"/>
       <c r="B29" s="2" t="s">
         <v>28</v>
       </c>
       <c r="D29" s="8"/>
     </row>
     <row r="30" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8"/>
       <c r="B30" s="2" t="s">
         <v>32</v>
       </c>
       <c r="D30" s="8"/>
       <c r="E30" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="8"/>
       <c r="B31" s="2" t="s">
         <v>27</v>
       </c>
       <c r="D31" s="8"/>
     </row>
     <row r="32" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
+      <c r="A32" s="14"/>
       <c r="B32" s="6"/>
       <c r="C32" s="6"/>
       <c r="D32" s="14"/>
       <c r="E32" s="6"/>
     </row>
     <row r="33" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="6"/>
+      <c r="A33" s="14"/>
       <c r="B33" s="6"/>
       <c r="C33" s="6"/>
       <c r="D33" s="14"/>
       <c r="E33" s="6"/>
     </row>
     <row r="34" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="6"/>
+      <c r="A34" s="14"/>
       <c r="B34" s="6"/>
       <c r="C34" s="6"/>
       <c r="D34" s="14"/>
       <c r="E34" s="6"/>
     </row>
     <row r="35" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="6"/>
+      <c r="A35" s="14"/>
       <c r="B35" s="6"/>
       <c r="C35" s="6"/>
       <c r="D35" s="14"/>
       <c r="E35" s="6"/>
     </row>
     <row r="36" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="6"/>
+      <c r="A36" s="14"/>
       <c r="B36" s="6"/>
       <c r="C36" s="6"/>
       <c r="D36" s="14"/>
       <c r="E36" s="6"/>
     </row>
     <row r="37" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="6"/>
+      <c r="A37" s="14"/>
       <c r="B37" s="6"/>
       <c r="C37" s="6"/>
       <c r="D37" s="14"/>
       <c r="E37" s="6"/>
     </row>
     <row r="38" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="6"/>
+      <c r="A38" s="14"/>
       <c r="B38" s="6"/>
       <c r="C38" s="6"/>
       <c r="D38" s="14"/>
       <c r="E38" s="6"/>
     </row>
     <row r="39" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="6"/>
+      <c r="A39" s="14"/>
       <c r="B39" s="6"/>
       <c r="C39" s="6"/>
       <c r="D39" s="14"/>
       <c r="E39" s="6"/>
     </row>
     <row r="40" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="6"/>
+      <c r="A40" s="14"/>
       <c r="B40" s="6"/>
       <c r="C40" s="6"/>
       <c r="D40" s="14"/>
       <c r="E40" s="6"/>
     </row>
     <row r="41" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="6"/>
+      <c r="A41" s="14"/>
       <c r="B41" s="6"/>
       <c r="C41" s="6"/>
       <c r="D41" s="14"/>
       <c r="E41" s="6"/>
     </row>
     <row r="42" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="6"/>
+      <c r="A42" s="14"/>
       <c r="B42" s="6"/>
       <c r="C42" s="6"/>
       <c r="D42" s="14"/>
       <c r="E42" s="6"/>
     </row>
     <row r="43" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
+      <c r="A43" s="14"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
       <c r="D43" s="14"/>
       <c r="E43" s="6"/>
     </row>
     <row r="44" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="6"/>
+      <c r="A44" s="14"/>
       <c r="B44" s="6"/>
       <c r="C44" s="6"/>
       <c r="D44" s="14"/>
       <c r="E44" s="6"/>
     </row>
     <row r="45" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="6"/>
+      <c r="A45" s="14"/>
       <c r="B45" s="6"/>
       <c r="C45" s="6"/>
       <c r="D45" s="14"/>
       <c r="E45" s="6"/>
     </row>
     <row r="46" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="6"/>
+      <c r="A46" s="14"/>
       <c r="B46" s="6"/>
       <c r="C46" s="6"/>
       <c r="D46" s="14"/>
       <c r="E46" s="6"/>
     </row>
     <row r="47" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="6"/>
+      <c r="A47" s="14"/>
       <c r="B47" s="6"/>
       <c r="C47" s="6"/>
       <c r="D47" s="14"/>
       <c r="E47" s="6"/>
     </row>
     <row r="48" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="6"/>
+      <c r="A48" s="14"/>
       <c r="B48" s="6"/>
       <c r="C48" s="6"/>
       <c r="D48" s="14"/>
       <c r="E48" s="6"/>
     </row>
     <row r="49" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="6"/>
+      <c r="A49" s="14"/>
       <c r="B49" s="6"/>
       <c r="C49" s="6"/>
       <c r="D49" s="14"/>
       <c r="E49" s="6"/>
     </row>
     <row r="50" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="6"/>
+      <c r="A50" s="14"/>
       <c r="B50" s="6"/>
       <c r="C50" s="6"/>
       <c r="D50" s="14"/>
       <c r="E50" s="6"/>
     </row>
     <row r="51" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="6"/>
+      <c r="A51" s="14"/>
       <c r="B51" s="6"/>
       <c r="C51" s="6"/>
       <c r="D51" s="14"/>
       <c r="E51" s="6"/>
     </row>
     <row r="52" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="8"/>
       <c r="D52" s="8"/>
     </row>
     <row r="53" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="8"/>
       <c r="D53" s="8"/>
     </row>
     <row r="54" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="8"/>
       <c r="D54" s="8"/>
     </row>
     <row r="55" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="8"/>
       <c r="D55" s="8"/>
     </row>
     <row r="56" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="8"/>
       <c r="D56" s="8"/>
     </row>
     <row r="57" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="8"/>
       <c r="D57" s="8"/>
     </row>
     <row r="58" spans="1:5" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="8"/>
       <c r="D58" s="8"/>
     </row>
   </sheetData>
@@ -2147,8 +2177,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E29"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2203,34 +2233,18 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>141112206</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="4">
-        <v>85261775689</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>55</v>
-      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>141113619</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>39</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="4">
-        <v>82165152615</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>55</v>
-      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>

</xml_diff>

<commit_message>
Edit 'pesertaseleksidb.xlsx' -> Edit Tampilan.
</commit_message>
<xml_diff>
--- a/pesertaseleksidb.xlsx
+++ b/pesertaseleksidb.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\2. Janward Alfredo Situmorang\KMK\KMK 2015\panitiaseleksikmk2015\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="K:\mikroskil\kmkmikroskil\2015\panitiaseleksikmk2015\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9195"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="9195" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MENDAFTAR" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="107">
   <si>
     <t>Daftar Peserta Seleksi Pengurus UKM - KMK Mikroskil Medan Periode 2015/2016</t>
   </si>
@@ -143,12 +143,6 @@
   </si>
   <si>
     <t>DIUNDANG</t>
-  </si>
-  <si>
-    <t>Eben Roy Silalahi</t>
-  </si>
-  <si>
-    <t>Derly Matondang</t>
   </si>
   <si>
     <t>TI (2014)</t>
@@ -1347,8 +1341,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1379,7 +1375,7 @@
     </row>
     <row r="4" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
@@ -1405,13 +1401,13 @@
         <v>141113473</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1422,13 +1418,13 @@
         <v>132112018</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1439,13 +1435,13 @@
         <v>141110841</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1456,13 +1452,13 @@
         <v>141112974</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1473,13 +1469,13 @@
         <v>148111411</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="E9" s="8" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1490,13 +1486,13 @@
         <v>141114380</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1507,13 +1503,13 @@
         <v>141110736</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1524,13 +1520,13 @@
         <v>132112476</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1541,13 +1537,13 @@
         <v>132112964</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1558,13 +1554,13 @@
         <v>132113498</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1572,7 +1568,7 @@
         <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>9</v>
@@ -1592,14 +1588,14 @@
         <v>132112808</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D16" s="6"/>
       <c r="E16" s="14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1610,13 +1606,13 @@
         <v>148111136</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="E17" s="8" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1627,14 +1623,14 @@
         <v>132111101</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="D18" s="6"/>
       <c r="E18" s="14" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1642,16 +1638,16 @@
         <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="2" t="s">
+      <c r="E19" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="E19" s="8" t="s">
-        <v>51</v>
-      </c>
       <c r="F19" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1659,16 +1655,16 @@
         <v>16</v>
       </c>
       <c r="C20" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="E20" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="D20" s="13" t="s">
-        <v>80</v>
-      </c>
-      <c r="E20" s="8" t="s">
-        <v>81</v>
-      </c>
       <c r="F20" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1676,16 +1672,16 @@
         <v>17</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="E21" s="12" t="s">
         <v>48</v>
       </c>
-      <c r="E21" s="12" t="s">
-        <v>50</v>
-      </c>
       <c r="F21" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1696,13 +1692,13 @@
         <v>141113881</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1713,13 +1709,13 @@
         <v>142113061</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F23" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="F23" s="2" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1727,7 +1723,7 @@
         <v>20</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>6</v>
@@ -1747,13 +1743,13 @@
         <v>141114509</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1764,13 +1760,13 @@
         <v>141112583</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1781,13 +1777,13 @@
         <v>148111705</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1798,13 +1794,13 @@
         <v>142113771</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1815,13 +1811,13 @@
         <v>141114584</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1832,14 +1828,14 @@
         <v>132112859</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D30" s="6"/>
       <c r="E30" s="14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1850,13 +1846,13 @@
         <v>148111497</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1867,13 +1863,13 @@
         <v>148110459</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1980,8 +1976,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K58"/>
   <sheetViews>
-    <sheetView topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6:K6"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection activeCell="A4" sqref="A4"/>
+      <selection pane="bottomLeft" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1989,7 +1987,7 @@
     <col min="1" max="1" width="9.140625" style="1"/>
     <col min="2" max="2" width="14.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="35.42578125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="27.7109375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="39.28515625" style="1" customWidth="1"/>
     <col min="5" max="5" width="22.85546875" style="10" customWidth="1"/>
     <col min="6" max="6" width="24.5703125" style="1" customWidth="1"/>
     <col min="7" max="7" width="9.140625" style="1"/>
@@ -2014,7 +2012,7 @@
     </row>
     <row r="4" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
@@ -2041,7 +2039,7 @@
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2053,7 +2051,7 @@
       </c>
       <c r="E6" s="8"/>
       <c r="H6" s="18" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="I6" s="18"/>
       <c r="J6" s="18"/>
@@ -2068,10 +2066,10 @@
       </c>
       <c r="E7" s="8"/>
       <c r="H7" s="19" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
@@ -2081,7 +2079,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="E8" s="8"/>
       <c r="H8" s="19"/>
@@ -2109,13 +2107,13 @@
         <v>25</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2124,7 +2122,7 @@
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="14"/>
@@ -2154,7 +2152,7 @@
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="14"/>
@@ -2209,7 +2207,7 @@
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2315,7 +2313,7 @@
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2571,7 +2569,7 @@
   <dimension ref="A1:E29"/>
   <sheetViews>
     <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="E8" sqref="A5:E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2626,34 +2624,18 @@
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>141112206</v>
-      </c>
-      <c r="B5" s="2" t="s">
-        <v>40</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
       <c r="C5" s="3"/>
-      <c r="D5" s="4">
-        <v>85261775689</v>
-      </c>
-      <c r="E5" s="2" t="s">
-        <v>55</v>
-      </c>
+      <c r="D5" s="4"/>
+      <c r="E5" s="2"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>141113619</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>39</v>
-      </c>
+      <c r="A6" s="2"/>
+      <c r="B6" s="2"/>
       <c r="C6" s="3"/>
-      <c r="D6" s="4">
-        <v>82165152615</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>55</v>
-      </c>
+      <c r="D6" s="4"/>
+      <c r="E6" s="2"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="2"/>

</xml_diff>

<commit_message>
menambahkan data yang  mendaftar lewat email
</commit_message>
<xml_diff>
--- a/pesertaseleksidb.xlsx
+++ b/pesertaseleksidb.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="118">
   <si>
     <t>Daftar Peserta Seleksi Pengurus UKM - KMK Mikroskil Medan Periode 2015/2016</t>
   </si>
@@ -52,18 +52,12 @@
     <t>obbie.christian@gmail.com</t>
   </si>
   <si>
-    <t>081378458217</t>
-  </si>
-  <si>
     <t>Joel Adlino Pardede</t>
   </si>
   <si>
     <t>joeladlino26@yahoo.com</t>
   </si>
   <si>
-    <t>085372614506</t>
-  </si>
-  <si>
     <t>Wahana Ujung</t>
   </si>
   <si>
@@ -178,30 +172,18 @@
     <t>Lidya Veronica Hutabarat</t>
   </si>
   <si>
-    <t>082166562468</t>
-  </si>
-  <si>
-    <t>085762395411</t>
-  </si>
-  <si>
     <t>Riddik</t>
   </si>
   <si>
     <t>Nita Febrina Butar-butar</t>
   </si>
   <si>
-    <t>087744750232 / 082363963039</t>
-  </si>
-  <si>
     <t>Kamis 2 Juli 2015</t>
   </si>
   <si>
     <t>Sisilya Dewi Siregar</t>
   </si>
   <si>
-    <t>082276876382</t>
-  </si>
-  <si>
     <t>Wandiro.panggabean@hackermail.com</t>
   </si>
   <si>
@@ -211,99 +193,54 @@
     <t>Indah Priskila Butar-butar</t>
   </si>
   <si>
-    <t>081281128784</t>
-  </si>
-  <si>
     <t>Imelda Sadna Sianturi</t>
   </si>
   <si>
-    <t>082370246730 / 52770df0</t>
-  </si>
-  <si>
     <t>No</t>
   </si>
   <si>
     <t>Dahlia Agustina Purba</t>
   </si>
   <si>
-    <t>081263068983</t>
-  </si>
-  <si>
     <t>Fitriaman Lase</t>
   </si>
   <si>
-    <t>082272628901</t>
-  </si>
-  <si>
     <t>Andrian Sitinjak</t>
   </si>
   <si>
-    <t>081360127202</t>
-  </si>
-  <si>
     <t>Pransisco Simatupang</t>
   </si>
   <si>
-    <t>081287940531</t>
-  </si>
-  <si>
     <t>Sri Astuti Sihotang</t>
   </si>
   <si>
-    <t>083199779933</t>
-  </si>
-  <si>
     <t>Endang Aprilin Siallagan</t>
   </si>
   <si>
-    <t>082276426833</t>
-  </si>
-  <si>
     <t>Ami Olivya Sibarani</t>
   </si>
   <si>
-    <t>085297462566</t>
-  </si>
-  <si>
     <t>Lihardo Rawaja Haloho</t>
   </si>
   <si>
     <t>haloholihardo@gmail.com</t>
   </si>
   <si>
-    <t>082276845356</t>
-  </si>
-  <si>
     <t>Ruben Siburian</t>
   </si>
   <si>
-    <t>089622656574</t>
-  </si>
-  <si>
     <t>Yuliana Siahaan</t>
   </si>
   <si>
-    <t>085372781233</t>
-  </si>
-  <si>
     <t>Shinta warni Meliala</t>
   </si>
   <si>
-    <t>085761761106</t>
-  </si>
-  <si>
     <t>Dian Kristin Silaban</t>
   </si>
   <si>
-    <t>085206514334</t>
-  </si>
-  <si>
     <t>Widia Marito Manullang</t>
   </si>
   <si>
-    <t>082276099679</t>
-  </si>
-  <si>
     <t>Keterangan</t>
   </si>
   <si>
@@ -316,43 +253,133 @@
     <t>Natalya Uli Purba</t>
   </si>
   <si>
-    <t>082273350631</t>
-  </si>
-  <si>
     <t>Juni Susanti Siregar</t>
   </si>
   <si>
-    <t>082272756482</t>
-  </si>
-  <si>
     <t>Ines Lidwina Damanik</t>
   </si>
   <si>
-    <t>085760260603</t>
-  </si>
-  <si>
     <t>Anaria Novitasari Sitio</t>
   </si>
   <si>
-    <t>081269576256</t>
-  </si>
-  <si>
     <t>Surya Simarmata</t>
   </si>
   <si>
-    <t>085763552786</t>
-  </si>
-  <si>
     <t>Johannes Putra Rezeki Sianturi</t>
   </si>
   <si>
-    <t>081265361098</t>
-  </si>
-  <si>
     <t>Kevin Julianto Alexander Pane</t>
   </si>
   <si>
-    <t>081262958404</t>
+    <t>Maradona Jonas Simanullang</t>
+  </si>
+  <si>
+    <t>AGUSTINA DESI RATNASARI</t>
+  </si>
+  <si>
+    <t>0852-9634-2216</t>
+  </si>
+  <si>
+    <t>0822-7642-0001</t>
+  </si>
+  <si>
+    <t>0852-9746-2566</t>
+  </si>
+  <si>
+    <t>0812-6957-6256</t>
+  </si>
+  <si>
+    <t>0813-6012-7202</t>
+  </si>
+  <si>
+    <t>0812-6306-8983</t>
+  </si>
+  <si>
+    <t>0852-0651-4334</t>
+  </si>
+  <si>
+    <t>0822-7642-6833</t>
+  </si>
+  <si>
+    <t>0822-7262-8901</t>
+  </si>
+  <si>
+    <t>0823-7024-6730 / 52770df0</t>
+  </si>
+  <si>
+    <t>0812-8112-8784</t>
+  </si>
+  <si>
+    <t>0857-6026-0603</t>
+  </si>
+  <si>
+    <t>0853-7261-4506</t>
+  </si>
+  <si>
+    <t>0812-6536-1098</t>
+  </si>
+  <si>
+    <t>0822-7275-6482</t>
+  </si>
+  <si>
+    <t>0812-6295-8404</t>
+  </si>
+  <si>
+    <t>0857-6239-5411</t>
+  </si>
+  <si>
+    <t>0822-7684-5356</t>
+  </si>
+  <si>
+    <t>0821-6656-2468</t>
+  </si>
+  <si>
+    <t>0822-7335-0631</t>
+  </si>
+  <si>
+    <t>08774475-0232 / 0823-6396-3039</t>
+  </si>
+  <si>
+    <t>0813-7845-8217</t>
+  </si>
+  <si>
+    <t>0812-8794-0531</t>
+  </si>
+  <si>
+    <t>0896-2265-6574</t>
+  </si>
+  <si>
+    <t>0857-6176-1106</t>
+  </si>
+  <si>
+    <t>0822-7687-6382</t>
+  </si>
+  <si>
+    <t>0831-9977-9933</t>
+  </si>
+  <si>
+    <t>0857-6355-2786</t>
+  </si>
+  <si>
+    <t>0822-7609-9679</t>
+  </si>
+  <si>
+    <t>0853-7278-1233</t>
+  </si>
+  <si>
+    <t>Dewi S Panjaitan</t>
+  </si>
+  <si>
+    <t>0823-6524-4833</t>
+  </si>
+  <si>
+    <t>Sarmapanjaitan@gmail.com</t>
+  </si>
+  <si>
+    <t>Alfrido Nezer Panggabean</t>
+  </si>
+  <si>
+    <t>0823-6465-8673</t>
   </si>
 </sst>
 </file>
@@ -1012,8 +1039,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:F33" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
-  <autoFilter ref="B4:F33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="B4:F36" totalsRowShown="0" headerRowDxfId="26" dataDxfId="25">
+  <autoFilter ref="B4:F36"/>
   <sortState ref="B5:F33">
     <sortCondition ref="C4:C33"/>
   </sortState>
@@ -1029,8 +1056,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A4:A33" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
-  <autoFilter ref="A4:A33"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="4" name="Table4" displayName="Table4" ref="A4:A36" totalsRowShown="0" headerRowDxfId="19" dataDxfId="18">
+  <autoFilter ref="A4:A36"/>
   <tableColumns count="1">
     <tableColumn id="1" name="No" dataDxfId="17"/>
   </tableColumns>
@@ -1347,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F58"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="C32" sqref="C32"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F34" sqref="F34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1370,7 +1397,7 @@
     </row>
     <row r="2" spans="1:6" s="5" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="E2" s="9"/>
     </row>
@@ -1379,7 +1406,7 @@
     </row>
     <row r="4" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
@@ -1405,13 +1432,13 @@
         <v>141113473</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>77</v>
+        <v>63</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>78</v>
+        <v>85</v>
       </c>
       <c r="F5" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1422,13 +1449,13 @@
         <v>132112018</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="E6" s="8" t="s">
-        <v>102</v>
+        <v>86</v>
       </c>
       <c r="F6" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1439,13 +1466,13 @@
         <v>141110841</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="F7" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="8" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1456,13 +1483,13 @@
         <v>141112974</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="E8" s="8" t="s">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1473,13 +1500,13 @@
         <v>148111411</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>89</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1490,13 +1517,13 @@
         <v>141114380</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>75</v>
+        <v>62</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>76</v>
+        <v>90</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1507,13 +1534,13 @@
         <v>141110736</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="E11" s="8" t="s">
-        <v>68</v>
+        <v>91</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="12" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1524,13 +1551,13 @@
         <v>132112476</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="E12" s="8" t="s">
-        <v>63</v>
+        <v>92</v>
       </c>
       <c r="F12" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1541,13 +1568,13 @@
         <v>132112964</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E13" s="8" t="s">
-        <v>61</v>
+        <v>93</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1558,13 +1585,13 @@
         <v>132113498</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>99</v>
+        <v>76</v>
       </c>
       <c r="E14" s="8" t="s">
-        <v>100</v>
+        <v>94</v>
       </c>
       <c r="F14" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="15" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1572,16 +1599,16 @@
         <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="D15" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D15" s="3" t="s">
-        <v>10</v>
-      </c>
       <c r="E15" s="11" t="s">
-        <v>11</v>
+        <v>95</v>
       </c>
     </row>
     <row r="16" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1592,14 +1619,14 @@
         <v>132112808</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>105</v>
+        <v>79</v>
       </c>
       <c r="D16" s="6"/>
-      <c r="E16" s="14" t="s">
-        <v>106</v>
+      <c r="E16" s="8" t="s">
+        <v>96</v>
       </c>
       <c r="F16" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="17" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1610,13 +1637,13 @@
         <v>148111136</v>
       </c>
       <c r="C17" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E17" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="E17" s="8" t="s">
-        <v>98</v>
-      </c>
       <c r="F17" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1627,14 +1654,14 @@
         <v>132111101</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>107</v>
+        <v>80</v>
       </c>
       <c r="D18" s="6"/>
-      <c r="E18" s="14" t="s">
-        <v>108</v>
+      <c r="E18" s="8" t="s">
+        <v>98</v>
       </c>
       <c r="F18" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="19" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1642,16 +1669,16 @@
         <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>49</v>
-      </c>
       <c r="E19" s="8" t="s">
-        <v>51</v>
+        <v>99</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1659,16 +1686,16 @@
         <v>16</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>79</v>
+        <v>64</v>
       </c>
       <c r="D20" s="13" t="s">
-        <v>80</v>
+        <v>65</v>
       </c>
       <c r="E20" s="8" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="F20" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="21" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1676,16 +1703,16 @@
         <v>17</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E21" s="12" t="s">
-        <v>50</v>
+        <v>101</v>
       </c>
       <c r="F21" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1696,13 +1723,13 @@
         <v>141113881</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>95</v>
+        <v>74</v>
       </c>
       <c r="E22" s="8" t="s">
-        <v>96</v>
+        <v>102</v>
       </c>
       <c r="F22" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="23" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1713,13 +1740,13 @@
         <v>142113061</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="E23" s="8" t="s">
-        <v>54</v>
+        <v>103</v>
       </c>
       <c r="F23" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="24" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1727,7 +1754,7 @@
         <v>20</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>6</v>
@@ -1736,7 +1763,7 @@
         <v>7</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>8</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1747,13 +1774,13 @@
         <v>141114509</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>71</v>
+        <v>60</v>
       </c>
       <c r="E25" s="8" t="s">
-        <v>72</v>
+        <v>105</v>
       </c>
       <c r="F25" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="26" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1764,13 +1791,13 @@
         <v>141112583</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>82</v>
+        <v>66</v>
       </c>
       <c r="E26" s="8" t="s">
-        <v>83</v>
+        <v>106</v>
       </c>
       <c r="F26" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="27" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1781,13 +1808,13 @@
         <v>148111705</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>86</v>
+        <v>68</v>
       </c>
       <c r="E27" s="8" t="s">
-        <v>87</v>
+        <v>107</v>
       </c>
       <c r="F27" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1798,13 +1825,13 @@
         <v>142113771</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
       <c r="E28" s="8" t="s">
-        <v>57</v>
+        <v>108</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="29" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1815,13 +1842,13 @@
         <v>141114584</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="E29" s="8" t="s">
-        <v>74</v>
+        <v>109</v>
       </c>
       <c r="F29" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="30" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1832,14 +1859,14 @@
         <v>132112859</v>
       </c>
       <c r="C30" s="6" t="s">
-        <v>103</v>
+        <v>78</v>
       </c>
       <c r="D30" s="6"/>
-      <c r="E30" s="14" t="s">
-        <v>104</v>
+      <c r="E30" s="8" t="s">
+        <v>110</v>
       </c>
       <c r="F30" s="6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1850,13 +1877,13 @@
         <v>148111497</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="E31" s="8" t="s">
-        <v>91</v>
+        <v>111</v>
       </c>
       <c r="F31" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="32" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1867,33 +1894,74 @@
         <v>148110459</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>84</v>
+        <v>67</v>
       </c>
       <c r="E32" s="8" t="s">
-        <v>85</v>
+        <v>112</v>
       </c>
       <c r="F32" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="33" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>29</v>
       </c>
-      <c r="B33" s="6"/>
-      <c r="C33" s="6"/>
+      <c r="B33" s="6">
+        <v>141112729</v>
+      </c>
+      <c r="C33" s="6" t="s">
+        <v>81</v>
+      </c>
       <c r="D33" s="6"/>
-      <c r="E33" s="14"/>
-      <c r="F33" s="6"/>
-    </row>
-    <row r="34" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E34" s="8"/>
-    </row>
-    <row r="35" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E35" s="8"/>
+      <c r="E33" s="8" t="s">
+        <v>84</v>
+      </c>
+      <c r="F33" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A34" s="2">
+        <v>30</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E34" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A35" s="2">
+        <v>31</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D35" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="E35" s="1" t="s">
+        <v>114</v>
+      </c>
     </row>
     <row r="36" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E36" s="8"/>
+      <c r="A36" s="2">
+        <v>32</v>
+      </c>
+      <c r="B36" s="2">
+        <v>131110658</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>116</v>
+      </c>
+      <c r="E36" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="37" spans="1:6" s="2" customFormat="1" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E37" s="8"/>
@@ -2005,7 +2073,7 @@
     </row>
     <row r="2" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="5" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="E2" s="8"/>
     </row>
@@ -2014,7 +2082,7 @@
     </row>
     <row r="4" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>64</v>
+        <v>56</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>1</v>
@@ -2037,11 +2105,11 @@
         <v>1</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E5" s="8"/>
       <c r="F5" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2049,11 +2117,11 @@
         <v>2</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="E6" s="8"/>
       <c r="H6" s="18" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="I6" s="18"/>
       <c r="J6" s="18"/>
@@ -2064,14 +2132,14 @@
         <v>3</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="E7" s="8"/>
       <c r="H7" s="19" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="I7" s="20" t="s">
-        <v>94</v>
+        <v>73</v>
       </c>
       <c r="J7" s="20"/>
       <c r="K7" s="20"/>
@@ -2081,7 +2149,7 @@
         <v>4</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>52</v>
+        <v>48</v>
       </c>
       <c r="E8" s="8"/>
       <c r="H8" s="19"/>
@@ -2094,7 +2162,7 @@
         <v>5</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="E9" s="8"/>
     </row>
@@ -2106,16 +2174,16 @@
         <v>141113759</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D10" s="13" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="E10" s="8" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2124,7 +2192,7 @@
       </c>
       <c r="B11" s="6"/>
       <c r="C11" s="6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D11" s="6"/>
       <c r="E11" s="14"/>
@@ -2135,7 +2203,7 @@
         <v>8</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="E12" s="8"/>
     </row>
@@ -2144,7 +2212,7 @@
         <v>9</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E13" s="8"/>
     </row>
@@ -2154,7 +2222,7 @@
       </c>
       <c r="B14" s="6"/>
       <c r="C14" s="6" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D14" s="6"/>
       <c r="E14" s="14"/>
@@ -2165,7 +2233,7 @@
         <v>11</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E15" s="8"/>
     </row>
@@ -2174,7 +2242,7 @@
         <v>12</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D16" s="3"/>
       <c r="E16" s="15"/>
@@ -2184,7 +2252,7 @@
         <v>13</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="E17" s="8"/>
     </row>
@@ -2194,7 +2262,7 @@
       </c>
       <c r="B18" s="16"/>
       <c r="C18" s="16" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D18" s="16"/>
       <c r="E18" s="17"/>
@@ -2205,11 +2273,11 @@
         <v>15</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E19" s="8"/>
       <c r="F19" s="7" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="20" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2218,7 +2286,7 @@
       </c>
       <c r="B20" s="16"/>
       <c r="C20" s="16" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D20" s="16"/>
       <c r="E20" s="17"/>
@@ -2229,7 +2297,7 @@
         <v>17</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="E21" s="8"/>
     </row>
@@ -2238,7 +2306,7 @@
         <v>18</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E22" s="8"/>
     </row>
@@ -2247,7 +2315,7 @@
         <v>19</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="E23" s="8"/>
     </row>
@@ -2256,7 +2324,7 @@
         <v>20</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="E24" s="8"/>
     </row>
@@ -2265,7 +2333,7 @@
         <v>21</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="E25" s="8"/>
     </row>
@@ -2274,7 +2342,7 @@
         <v>22</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E26" s="8"/>
     </row>
@@ -2283,7 +2351,7 @@
         <v>23</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E27" s="8"/>
     </row>
@@ -2292,7 +2360,7 @@
         <v>24</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="15"/>
@@ -2302,7 +2370,7 @@
         <v>25</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="E29" s="8"/>
     </row>
@@ -2311,11 +2379,11 @@
         <v>26</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E30" s="8"/>
       <c r="F30" s="2" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:6" s="2" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.25">
@@ -2323,7 +2391,7 @@
         <v>27</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="E31" s="8"/>
     </row>
@@ -2594,7 +2662,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
@@ -2630,14 +2698,14 @@
         <v>141112206</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="4">
         <v>85261775689</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -2645,14 +2713,14 @@
         <v>141113619</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="4">
         <v>82165152615</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>55</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>